<commit_message>
Added body type classify
</commit_message>
<xml_diff>
--- a/MealPlan.xlsx
+++ b/MealPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shehan\Documents\Projects\HerbalProject\BodyFatEst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A43E55B-77AC-40BD-ACF1-524314FF1EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D57D520-6068-41F7-9D29-F4207D9D2E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{A795B1B8-DE4F-40CF-A72C-6EDD6B85480B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{A795B1B8-DE4F-40CF-A72C-6EDD6B85480B}"/>
   </bookViews>
   <sheets>
     <sheet name="Diabetes" sheetId="1" r:id="rId1"/>
@@ -692,9 +692,6 @@
     <t>Body Types</t>
   </si>
   <si>
-    <t>Ectomorph Type</t>
-  </si>
-  <si>
     <t>Fried Beans Curry 50g</t>
   </si>
   <si>
@@ -702,6 +699,9 @@
   </si>
   <si>
     <t>Mesomorph</t>
+  </si>
+  <si>
+    <t>Ectomorph</t>
   </si>
 </sst>
 </file>
@@ -1103,19 +1103,19 @@
       <selection activeCell="H18" sqref="H16:H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>60</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="C5" t="s">
         <v>6</v>
@@ -1202,13 +1202,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="C8" t="s">
         <v>50</v>
@@ -1232,7 +1232,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="C10" t="s">
         <v>121</v>
@@ -1282,7 +1282,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="C11" t="s">
         <v>122</v>
@@ -1306,7 +1306,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="C12" t="s">
         <v>2</v>
@@ -1330,7 +1330,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>3</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="C17" t="s">
         <v>62</v>
@@ -1391,21 +1391,21 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="G18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="C24" t="s">
         <v>65</v>
@@ -1455,7 +1455,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="C25" t="s">
         <v>66</v>
@@ -1479,7 +1479,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="C26" t="s">
         <v>69</v>
@@ -1497,7 +1497,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="E27" t="s">
         <v>74</v>
@@ -1506,7 +1506,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="C30" t="s">
         <v>15</v>
@@ -1556,7 +1556,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="C31" t="s">
         <v>87</v>
@@ -1580,7 +1580,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>88</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>90</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="C37" t="s">
         <v>110</v>
@@ -1670,7 +1670,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>109</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>63</v>
       </c>
@@ -1704,19 +1704,19 @@
       <selection activeCell="E40" sqref="E38:E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" customWidth="1"/>
-    <col min="6" max="6" width="23.88671875" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" customWidth="1"/>
-    <col min="8" max="8" width="28.88671875" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>130</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" t="s">
         <v>9</v>
@@ -1778,19 +1778,19 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>50</v>
@@ -1814,7 +1814,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>132</v>
@@ -1838,7 +1838,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>2</v>
@@ -1888,7 +1888,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>137</v>
@@ -1912,7 +1912,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="C16" t="s">
         <v>56</v>
@@ -1933,7 +1933,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1960,23 +1960,23 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="E18" t="s">
         <v>49</v>
       </c>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
         <v>65</v>
@@ -2026,7 +2026,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" t="s">
         <v>79</v>
@@ -2050,7 +2050,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" t="s">
         <v>69</v>
@@ -2068,13 +2068,13 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="D29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
         <v>15</v>
@@ -2124,7 +2124,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" t="s">
         <v>87</v>
@@ -2148,7 +2148,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>154</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>90</v>
       </c>
@@ -2194,12 +2194,12 @@
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>110</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>109</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>155</v>
       </c>
@@ -2282,19 +2282,19 @@
       <selection activeCell="E13" sqref="E8:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" customWidth="1"/>
-    <col min="7" max="7" width="23.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>164</v>
       </c>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2347,22 +2347,22 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="C4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>50</v>
@@ -2386,7 +2386,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>132</v>
@@ -2410,7 +2410,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>145</v>
@@ -2460,7 +2460,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>202</v>
@@ -2484,7 +2484,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>137</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="C16" t="s">
         <v>47</v>
@@ -2522,7 +2522,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="C18" t="s">
         <v>49</v>
@@ -2565,19 +2565,19 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" customWidth="1"/>
-    <col min="7" max="7" width="24.21875" customWidth="1"/>
-    <col min="8" max="8" width="29.21875" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>177</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2629,19 +2629,19 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>50</v>
@@ -2665,7 +2665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>194</v>
@@ -2689,7 +2689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>145</v>
@@ -2739,7 +2739,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>185</v>
@@ -2763,7 +2763,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>198</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>56</v>
@@ -2804,7 +2804,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
         <v>49</v>
       </c>
@@ -2839,15 +2839,15 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>205</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>206</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>63</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>213</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>28</v>
       </c>
@@ -2902,17 +2902,17 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>209</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>81</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>82</v>
       </c>
@@ -2945,17 +2945,17 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>207</v>
       </c>
@@ -2969,7 +2969,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>26</v>
       </c>
@@ -2980,22 +2980,22 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>208</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>152</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>35</v>
       </c>
@@ -3025,22 +3025,22 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>210</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>143</v>
       </c>
@@ -3062,12 +3062,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>36</v>
       </c>
@@ -3079,21 +3079,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C607624-7596-44C1-AEC7-6C15A3386F15}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>216</v>
       </c>
@@ -3107,147 +3107,147 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>217</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" t="s">
         <v>64</v>
       </c>
-      <c r="C5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="C8" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>65</v>
       </c>
-      <c r="C6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="C9" t="s">
         <v>79</v>
       </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="D9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>69</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>220</v>
-      </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
       <c r="C14" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>79</v>
-      </c>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>69</v>
-      </c>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>219</v>
-      </c>
-      <c r="B23" t="s">
-        <v>151</v>
-      </c>
-      <c r="C23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>152</v>
-      </c>
-      <c r="D24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>